<commit_message>
mise à jour des backlogs et assignation des sprints
</commit_message>
<xml_diff>
--- a/doc/backLog/backlog_infra_V1.xlsx
+++ b/doc/backLog/backlog_infra_V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://auvencecom-my.sharepoint.com/personal/jonathan_berenguer_ynov_com/Documents/B2/Projet_uf/ProjetUF2020_2021/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://auvencecom-my.sharepoint.com/personal/jonathan_berenguer_ynov_com/Documents/B2/Projet_uf/ProjetUF2020_2021/doc/backLog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{38BF9074-37DF-4142-9CD7-540378877D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A9970242-9429-4CD0-AC8E-30A5A8786F97}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{38BF9074-37DF-4142-9CD7-540378877D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0016E3FD-EF7F-4E78-A4FC-0B05DFA2A877}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{288C5752-F91D-4169-A5AA-D5AD8174C2FD}"/>
+    <workbookView xWindow="348" yWindow="1068" windowWidth="17280" windowHeight="9420" xr2:uid="{288C5752-F91D-4169-A5AA-D5AD8174C2FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>User story créée</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>difficulté</t>
-  </si>
-  <si>
-    <t>na</t>
   </si>
   <si>
     <t>la connexion entre les différents pôles du projet doit être sécurisée</t>
@@ -458,7 +455,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,13 +493,13 @@
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -513,19 +510,19 @@
       <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
+      <c r="G2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -536,19 +533,19 @@
       <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
-        <v>9</v>
+      <c r="G3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>100</v>
@@ -559,31 +556,31 @@
       <c r="F4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
-        <v>9</v>
+      <c r="G4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
-        <v>9</v>
+      <c r="G5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -596,18 +593,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -759,14 +756,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C58DAF85-4393-489B-8E03-55F5E1DA6BF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86467EE2-8D7F-43A3-B629-3DC5F34CD41A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -778,6 +767,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C58DAF85-4393-489B-8E03-55F5E1DA6BF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
mise a jour doc
</commit_message>
<xml_diff>
--- a/doc/backLog/backlog_infra_V1.xlsx
+++ b/doc/backLog/backlog_infra_V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://auvencecom-my.sharepoint.com/personal/jonathan_berenguer_ynov_com/Documents/B2/Projet_uf/ProjetUF2020_2021/doc/backLog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clément\Desktop\dev\ynov\ProjetUF2020_2021\doc\backLog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{38BF9074-37DF-4142-9CD7-540378877D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0016E3FD-EF7F-4E78-A4FC-0B05DFA2A877}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E149ACC4-C0D4-460F-ADF7-0D20B04D46E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="1068" windowWidth="17280" windowHeight="9420" xr2:uid="{288C5752-F91D-4169-A5AA-D5AD8174C2FD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{288C5752-F91D-4169-A5AA-D5AD8174C2FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -114,10 +114,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -156,7 +159,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -452,136 +455,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B748B5-E75E-455A-825F-29C2F7C6913A}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.5546875" customWidth="1"/>
-    <col min="2" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" customWidth="1"/>
+    <col min="1" max="1" width="40.54296875" customWidth="1"/>
+    <col min="2" max="3" width="18.08984375" customWidth="1"/>
+    <col min="4" max="4" width="19.08984375" customWidth="1"/>
+    <col min="5" max="5" width="18.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="7" max="7" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>100</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>90</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>3</v>
       </c>
+      <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>100</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>70</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>2</v>
       </c>
+      <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>100</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>50</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>2</v>
       </c>
+      <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>3</v>
       </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -593,18 +628,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -756,6 +791,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C58DAF85-4393-489B-8E03-55F5E1DA6BF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86467EE2-8D7F-43A3-B629-3DC5F34CD41A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -767,14 +810,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C58DAF85-4393-489B-8E03-55F5E1DA6BF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>